<commit_message>
modified codebase, updated arbeitszeiten
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\revontulet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED56CBA1-0951-43FE-BC1F-9A9ACD5E449B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B12ACD-5031-4157-B22D-A5FF8C35B8EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Konzept Weiterarbeit</t>
+  </si>
+  <si>
+    <t>GitHub Repo erstellt</t>
+  </si>
+  <si>
+    <t>Code-Basis erstellt</t>
   </si>
 </sst>
 </file>
@@ -401,15 +407,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="B1:F7"/>
+  <dimension ref="B1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -451,6 +458,28 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>43497</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>43500</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added bt library support
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\revontulet\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B12ACD-5031-4157-B22D-A5FF8C35B8EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8269BF0-5767-45B0-9AD8-012938768FC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -42,12 +48,6 @@
     <t>Recherche, Konzept Erstellung</t>
   </si>
   <si>
-    <t>2 Stunden</t>
-  </si>
-  <si>
-    <t>1 Stunden</t>
-  </si>
-  <si>
     <t>Konzept Weiterarbeit</t>
   </si>
   <si>
@@ -55,6 +55,51 @@
   </si>
   <si>
     <t>Code-Basis erstellt</t>
+  </si>
+  <si>
+    <t>Änderungen am Code, Namen</t>
+  </si>
+  <si>
+    <t>Erstellen der Dokumentation</t>
+  </si>
+  <si>
+    <t>Einheit</t>
+  </si>
+  <si>
+    <t>Stunden</t>
+  </si>
+  <si>
+    <t>Summe der Stunden:</t>
+  </si>
+  <si>
+    <t>Arbeitszeit pro Tag</t>
+  </si>
+  <si>
+    <t>Anlegen des Projektmanagements in Trello</t>
+  </si>
+  <si>
+    <t>Diplomarbeitsbesprechung</t>
+  </si>
+  <si>
+    <t>Statusbericht</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Programmieren</t>
+  </si>
+  <si>
+    <t>genau</t>
+  </si>
+  <si>
+    <t>Bt Bibliothek über Maven hinzugefügt</t>
+  </si>
+  <si>
+    <t>Erste Versuche in der IDE mit fremden Librarys</t>
+  </si>
+  <si>
+    <t>Statusbericht geschrieben</t>
   </si>
 </sst>
 </file>
@@ -407,77 +452,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="B1:F9"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="55.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="37.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="1">
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <f>SUM(H:H)</f>
+        <v>18.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1">
         <v>43477</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
+        <v>36.844106463878326</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>43484</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <v>43497</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <v>43500</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G10" s="1">
+        <v>43509</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <v>43634</v>
+      </c>
+      <c r="H11">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="1">
-        <v>43484</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="1">
-        <v>43497</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="1">
-        <v>43500</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <v>43641</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <v>43642</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <v>43647</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <v>43654</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G16" s="1">
+        <v>43660</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G17" s="1">
+        <v>43661</v>
+      </c>
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created some classes and testui for testing
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8269BF0-5767-45B0-9AD8-012938768FC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20A5589-28E0-4053-A914-D694A84255FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>Statusbericht geschrieben</t>
+  </si>
+  <si>
+    <t>Dokumentation, Statusbericht</t>
+  </si>
+  <si>
+    <t>Recherche</t>
+  </si>
+  <si>
+    <t>Klassen und Bibilotheken in IntelliJ IDEA</t>
+  </si>
+  <si>
+    <t>Apache Ant</t>
+  </si>
+  <si>
+    <t>Erstellen neuer Klassen, Package testui zum Testen</t>
   </si>
 </sst>
 </file>
@@ -452,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +509,7 @@
       </c>
       <c r="B6">
         <f>SUM(H:H)</f>
-        <v>18.5</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -518,7 +533,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>36.844106463878326</v>
+        <v>36.887159533073934</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -683,6 +698,68 @@
       </c>
       <c r="K17" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G18" s="1">
+        <v>43662</v>
+      </c>
+      <c r="H18">
+        <v>0.75</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G19" s="1">
+        <v>43664</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G20" s="1">
+        <v>43666</v>
+      </c>
+      <c r="H20">
+        <v>0.75</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G21" s="1">
+        <v>43667</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes and additions in testui
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20A5589-28E0-4053-A914-D694A84255FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0C833E-DF6B-4DDB-A796-5464B7A303A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +509,7 @@
       </c>
       <c r="B6">
         <f>SUM(H:H)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -533,7 +533,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>36.887159533073934</v>
+        <v>36.653696498054479</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -750,7 +750,7 @@
         <v>43667</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
expanded Streamclient.java, added powershell folder
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0946016-E201-40BB-98F2-9FA59CBF6731}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3821F62-7F54-4C8B-8FC4-5B12AD20BCE9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>Implementation der ttorrent Bibiliothek</t>
+  </si>
+  <si>
+    <t>Schwierigkeiten bei der Implementierung der Bt Bibliothek</t>
+  </si>
+  <si>
+    <t>Hauptsächlich Dokumentation der vorhergegangenen Programmiertätigkeit</t>
+  </si>
+  <si>
+    <t>Erweiterung der StreamClient Klasse</t>
+  </si>
+  <si>
+    <t>Erstellen eines PS Scripts, siehe vorheriger Eintrag</t>
   </si>
 </sst>
 </file>
@@ -476,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +530,7 @@
       </c>
       <c r="B6">
         <f>SUM(H:H)</f>
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -542,7 +554,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>37.016129032258064</v>
+        <v>36.5</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -803,6 +815,88 @@
       </c>
       <c r="K23" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G24" s="1">
+        <v>43679</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" t="s">
+        <v>18</v>
+      </c>
+      <c r="K24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G25" s="1">
+        <v>43680</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G26" s="1">
+        <v>43681</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G27" s="1">
+        <v>43682</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>18</v>
+      </c>
+      <c r="K27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G28" s="1">
+        <v>43683</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filled in working form
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A70912-765B-4A7B-9568-0D63E68BF9E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C83F5A5-308D-48BC-9C39-68F3CD39EA0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Ausarbeitung der Client-Klassen</t>
+  </si>
+  <si>
+    <t>Lösen von Dependency Fehlern</t>
   </si>
 </sst>
 </file>
@@ -512,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +558,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -579,7 +582,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>32.820512820512825</v>
+        <v>32.446351931330476</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -600,7 +603,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>4.7407407407407414</v>
+        <v>4.8461538461538458</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -621,7 +624,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>4</v>
+        <v>4.0769230769230766</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1038,6 +1041,23 @@
       </c>
       <c r="I34" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="1">
+        <v>43691</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked on torrent hashing methods
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C83F5A5-308D-48BC-9C39-68F3CD39EA0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FED0153-5BD3-4119-898F-FD91D06C15FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>Lösen von Dependency Fehlern</t>
+  </si>
+  <si>
+    <t>Logging, Bugfixing</t>
+  </si>
+  <si>
+    <t>Eruieren der Möglichkeiten der Hash-Umwandlung von Torrent-Dateien</t>
   </si>
 </sst>
 </file>
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +564,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -582,7 +588,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>32.446351931330476</v>
+        <v>30.649350649350652</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -603,7 +609,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>4.8461538461538458</v>
+        <v>4.916666666666667</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -624,7 +630,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>4.0769230769230766</v>
+        <v>4.083333333333333</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1058,6 +1064,40 @@
       </c>
       <c r="I35" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="1">
+        <v>43692</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E37" s="1">
+        <v>43693</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added provisionally (test-)settings window
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FED0153-5BD3-4119-898F-FD91D06C15FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F607FD-942F-4702-9CD6-681E8DA8121B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="47">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Eruieren der Möglichkeiten der Hash-Umwandlung von Torrent-Dateien</t>
+  </si>
+  <si>
+    <t>Design neuer Einstellungen Klasse</t>
   </si>
 </sst>
 </file>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +567,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -588,7 +591,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>30.649350649350652</v>
+        <v>29.473684210526315</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -609,7 +612,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>4.916666666666667</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -630,7 +633,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>4.083333333333333</v>
+        <v>4.3809523809523814</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1098,6 +1101,37 @@
       </c>
       <c r="I37" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E38" s="1">
+        <v>43694</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E39" s="1">
+        <v>43695</v>
+      </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
download faulty, working on fix
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC51B0B-B396-41F6-9F6F-4A0168B411B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45D9A07-E305-4726-9FF2-BCE5711E0F90}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>Testinterface in zwei Teile geteilt</t>
+  </si>
+  <si>
+    <t>Theorie</t>
+  </si>
+  <si>
+    <t>Logging optimiert, Teil 1</t>
+  </si>
+  <si>
+    <t>Nichts</t>
   </si>
 </sst>
 </file>
@@ -527,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +579,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -594,7 +603,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>29.07488986784141</v>
+        <v>26.756756756756758</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -615,7 +624,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>5.5</v>
+        <v>6.6</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -636,7 +645,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>4.5</v>
+        <v>5.2666666666666666</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1152,6 +1161,68 @@
       </c>
       <c r="I40" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E41" s="1">
+        <v>43697</v>
+      </c>
+      <c r="F41">
+        <v>4</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E42" s="1">
+        <v>43698</v>
+      </c>
+      <c r="F42">
+        <v>3</v>
+      </c>
+      <c r="G42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E43" s="1">
+        <v>43700</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E44" s="1">
+        <v>43701</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some javadoc, but german
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45D9A07-E305-4726-9FF2-BCE5711E0F90}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0992371F-7CBE-44A3-9F6F-67BBF7BAAF4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -536,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -603,7 +603,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>26.756756756756758</v>
+        <v>26.454545454545453</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -624,7 +624,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>6.6</v>
+        <v>7.4615384615384617</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -645,7 +645,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>5.2666666666666666</v>
+        <v>5.9230769230769234</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1223,6 +1223,34 @@
       </c>
       <c r="H44" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E45" s="1">
+        <v>43702</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E46" s="1">
+        <v>43704</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug, optimization required
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CF616E-EEDD-4A58-8730-D348BEC0A134}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FD2B56-B775-440C-A831-9149CCAE7CE4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -545,7 +545,7 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +585,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -609,7 +609,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>25.161290322580648</v>
+        <v>25.233644859813083</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -630,7 +630,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>9.1</v>
+        <v>12.857142857142858</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -651,7 +651,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>7.1</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1278,7 +1278,7 @@
         <v>43707</v>
       </c>
       <c r="F48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G48" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
working on logging bug
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FD2B56-B775-440C-A831-9149CCAE7CE4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FEB299-EEEC-4C92-AA9D-6D2358C651B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Bugfixing</t>
+  </si>
+  <si>
+    <t>Änderungen im Basis Code</t>
+  </si>
+  <si>
+    <t>Weiterführende Anpasseungen</t>
   </si>
 </sst>
 </file>
@@ -542,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +591,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -609,7 +615,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>25.233644859813083</v>
+        <v>23.714285714285712</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -630,7 +636,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>12.857142857142858</v>
+        <v>27.666666666666668</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -651,7 +657,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1288,6 +1294,40 @@
       </c>
       <c r="I48" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E49" s="1">
+        <v>43713</v>
+      </c>
+      <c r="F49">
+        <v>4</v>
+      </c>
+      <c r="G49" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E50" s="1">
+        <v>43714</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added "multiple"-selection property to lv
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC2B412-D64A-4F63-BC88-1C522AE8D07A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F97D44B-A0C6-41C1-AC10-E1BFB1D5E28D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="71">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>Lösen des Download-Errors</t>
+  </si>
+  <si>
+    <t>User Interface editiert und Download-Buttons hinzugefügt</t>
+  </si>
+  <si>
+    <t>Download-Methoden revidiert bzw. Code inspiziert</t>
+  </si>
+  <si>
+    <t>Weiterführende Arbeit am Benutzer-Interface, insbesondere an den Optionen</t>
+  </si>
+  <si>
+    <t>Arbeit am Teil "Theoretische Grundlagen"</t>
   </si>
 </sst>
 </file>
@@ -584,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="E52" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +640,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -652,7 +664,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>27.522935779816514</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -673,7 +685,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>-0.51020408163265307</v>
+        <v>-0.37383177570093457</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -694,7 +706,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>-0.30612244897959184</v>
+        <v>-0.18691588785046728</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1439,6 +1451,9 @@
       <c r="H55" t="s">
         <v>59</v>
       </c>
+      <c r="I55" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="56" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E56" s="1">
@@ -1453,6 +1468,9 @@
       <c r="H56" t="s">
         <v>60</v>
       </c>
+      <c r="I56" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="57" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E57" s="1">
@@ -1467,6 +1485,9 @@
       <c r="H57" t="s">
         <v>59</v>
       </c>
+      <c r="I57" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="58" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E58" s="1">
@@ -1481,6 +1502,9 @@
       <c r="H58" t="s">
         <v>61</v>
       </c>
+      <c r="I58" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="59" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E59" s="1">
@@ -1567,6 +1591,57 @@
       </c>
       <c r="H64" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E65" s="1">
+        <v>43821</v>
+      </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="G65" t="s">
+        <v>11</v>
+      </c>
+      <c r="H65" t="s">
+        <v>18</v>
+      </c>
+      <c r="I65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E66" s="1">
+        <v>43822</v>
+      </c>
+      <c r="F66">
+        <v>4</v>
+      </c>
+      <c r="G66" t="s">
+        <v>11</v>
+      </c>
+      <c r="H66" t="s">
+        <v>18</v>
+      </c>
+      <c r="I66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E67" s="1">
+        <v>43823</v>
+      </c>
+      <c r="F67">
+        <v>3</v>
+      </c>
+      <c r="G67" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" t="s">
+        <v>18</v>
+      </c>
+      <c r="I67" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up Stream-classes code
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9777240-CB37-40CB-B926-C6EC5DB7BCDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDBB495-21C6-4046-91AE-5FC529803601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
+    <workbookView xWindow="8010" yWindow="1305" windowWidth="13500" windowHeight="13470" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="74">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -249,7 +249,10 @@
     <t>Hinzufügen weiterer Optionen zur GUI-Oberfläche "Torrent hinzufügen"</t>
   </si>
   <si>
-    <t>Möglichkeit hinzugefügt einzelne Torrent-Parts zu wählen</t>
+    <t>Code Cleanup und Entfernen überflüssiger Methoden</t>
+  </si>
+  <si>
+    <t>Code Analyse hin zur weiteren Überführung in das UI Modell</t>
   </si>
 </sst>
 </file>
@@ -602,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E52" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +649,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -670,7 +673,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>19.591836734693874</v>
+        <v>18.75</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -691,7 +694,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>-0.29357798165137616</v>
+        <v>-0.27027027027027029</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -712,7 +715,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>-0.11009174311926606</v>
+        <v>-9.0090090090090086E-2</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1682,6 +1685,23 @@
       </c>
       <c r="I69" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E70" s="1">
+        <v>43827</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" t="s">
+        <v>18</v>
+      </c>
+      <c r="I70" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new fxml window plus controller
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66963BC2-E8E5-4BC2-8145-D93FCEBD2DBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B980A4-1683-4D13-9A34-D2AB0A3EC745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="78">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Beaschäftigung mit Logging, unter anderem mit den Funktionen von log4j2</t>
+  </si>
+  <si>
+    <t>Erstellen neuer Klassen zur um die einzelnen Dateien eines Torrents auf der GUI darstellen zu können</t>
   </si>
 </sst>
 </file>
@@ -614,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
       <selection activeCell="I73" sqref="I73"/>
@@ -658,7 +661,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -682,7 +685,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>14.042553191489361</v>
+        <v>12.258064516129034</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -703,7 +706,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>-0.19469026548672566</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -724,7 +727,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>-1.7699115044247784E-2</v>
+        <v>8.771929824561403E-3</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1745,6 +1748,23 @@
       </c>
       <c r="I72" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E73" s="1">
+        <v>43466</v>
+      </c>
+      <c r="F73">
+        <v>3</v>
+      </c>
+      <c r="G73" t="s">
+        <v>11</v>
+      </c>
+      <c r="H73" t="s">
+        <v>18</v>
+      </c>
+      <c r="I73" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added atomic reference to single part page
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B980A4-1683-4D13-9A34-D2AB0A3EC745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E25FB6-17DF-4FCF-8E5B-25B0E514E67B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="81">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -265,6 +265,15 @@
   </si>
   <si>
     <t>Erstellen neuer Klassen zur um die einzelnen Dateien eines Torrents auf der GUI darstellen zu können</t>
+  </si>
+  <si>
+    <t>Weitere bearbeitung des GUI und erstellung des neuen Fensters zur einzelnen Torrent-Auswahl</t>
+  </si>
+  <si>
+    <t>Implementierung des neuen Fensters und Fehlerbehandlung</t>
+  </si>
+  <si>
+    <t>Definition mathematischer Operationen und Code Review</t>
   </si>
 </sst>
 </file>
@@ -617,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+      <selection activeCell="H75" sqref="H75:H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +670,7 @@
       </c>
       <c r="B6">
         <f>SUM(F:F)</f>
-        <v>161</v>
+        <v>167.5</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -685,7 +694,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>12.258064516129034</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -706,7 +715,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f ca="1">(((180 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>-0.16666666666666666</v>
+        <v>-0.10683760683760683</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -727,7 +736,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">(((160 -B6)/(_xlfn.DAYS(DATE(2019,9,9), TODAY())))*60)/60</f>
-        <v>8.771929824561403E-3</v>
+        <v>6.4102564102564097E-2</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1765,6 +1774,57 @@
       </c>
       <c r="I73" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E74" s="1">
+        <v>43467</v>
+      </c>
+      <c r="F74">
+        <v>4</v>
+      </c>
+      <c r="G74" t="s">
+        <v>11</v>
+      </c>
+      <c r="H74" t="s">
+        <v>18</v>
+      </c>
+      <c r="I74" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E75" s="1">
+        <v>43468</v>
+      </c>
+      <c r="F75">
+        <v>2</v>
+      </c>
+      <c r="G75" t="s">
+        <v>11</v>
+      </c>
+      <c r="H75" t="s">
+        <v>18</v>
+      </c>
+      <c r="I75" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E76" s="1">
+        <v>43469</v>
+      </c>
+      <c r="F76">
+        <v>0.5</v>
+      </c>
+      <c r="G76" t="s">
+        <v>11</v>
+      </c>
+      <c r="H76" t="s">
+        <v>18</v>
+      </c>
+      <c r="I76" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up translator, added google cloud dependency
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Pichler.xlsx
+++ b/docs/Arbeitszeit_Pichler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichler Martin\Desktop\BlueSoft\Diplomarbeit\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD70BA75-CB10-4F6F-B4C9-05AE6528107D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4442CC4A-98C8-49E5-8545-B937C24FB59E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{5D4EAA49-2E6F-45DD-AE1A-C1B8F9FBF238}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitszeit_Original" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="87">
   <si>
     <t>Diplomarbeit Arbeitszeit Pichler Martin</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>Aufarbeiten von Konfigurations-Bugs</t>
+  </si>
+  <si>
+    <t>Arbeitszeiten angepasst + neu formatiert</t>
+  </si>
+  <si>
+    <t>Das Tagebuch über die Verrechnung der Arbeitszeiten wurde gewissenhaft revisiert und in eine lesbarere Formatierung überführt</t>
   </si>
 </sst>
 </file>
@@ -643,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799AB88A-C83E-4E1E-A662-BCEACC959896}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +715,7 @@
       </c>
       <c r="B7">
         <f ca="1">((180 -B6)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
-        <v>3.2530120481927711</v>
+        <v>3.2926829268292681</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -1886,12 +1892,1042 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A730B3-BB80-4C5E-B327-935BC24F7A8F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" customWidth="1"/>
+    <col min="5" max="5" width="100.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43718</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43719</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43720</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43723</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43725</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43726</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43728</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43729</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43731</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <f>SUM(B:B)</f>
+        <v>176.5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43732</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11">
+        <f ca="1">((180 -G10)/(_xlfn.DAYS(DATE(2020,4,3), TODAY())))*60</f>
+        <v>2.5609756097560976</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43733</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43734</v>
+      </c>
+      <c r="B13">
+        <v>0.75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43735</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43736</v>
+      </c>
+      <c r="B15">
+        <v>0.75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43738</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43740</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43741</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43742</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43748</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43750</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43752</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43755</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43757</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43759</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43763</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43765</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43766</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43768</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43772</v>
+      </c>
+      <c r="B30">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43776</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43777</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>43778</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>43779</v>
+      </c>
+      <c r="B34">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>43780</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43782</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43784</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>43785</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43787</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43789</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43792</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>43800</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43810</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43811</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43813</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43814</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43818</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43825</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43826</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43827</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43828</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43829</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43830</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43832</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43834</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43835</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43837</v>
+      </c>
+      <c r="B57">
+        <v>0.5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43838</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>43839</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" t="s">
+        <v>82</v>
+      </c>
+      <c r="E59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>43840</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" t="s">
+        <v>82</v>
+      </c>
+      <c r="E60" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43842</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" t="s">
+        <v>85</v>
+      </c>
+      <c r="E61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A37">
+    <sortCondition ref="A1:A37"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>